<commit_message>
bug 59983: correctly update shared formulas when shifting rows. Thanks to Luca Martini for the initial failing unit test with test file and Chiara Marcheschi for the patch
git-svn-id: https://svn.apache.org/repos/asf/poi/trunk@1782111 13f79535-47bb-0310-9956-ffa450edef68
</commit_message>
<xml_diff>
--- a/test-data/spreadsheet/TestShiftRowSharedFormula.xlsx
+++ b/test-data/spreadsheet/TestShiftRowSharedFormula.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lucamar\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\SVN\poi-3.15.tgk\test-data\spreadsheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -344,10 +344,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:E5"/>
+  <dimension ref="B2:E6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -402,6 +402,20 @@
         <v>18</v>
       </c>
     </row>
+    <row r="6" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C6">
+        <f>SUM(C3:C5)</f>
+        <v>23</v>
+      </c>
+      <c r="D6">
+        <f t="shared" ref="D6" si="1">SUM(D3:D5)</f>
+        <v>28</v>
+      </c>
+      <c r="E6">
+        <f t="shared" ref="E6" si="2">SUM(E3:E5)</f>
+        <v>33</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>